<commit_message>
Auto commit on 2025-06-23 21:44 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -17,6 +17,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">Kalibrasyonlar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frq</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -216,14 +248,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A4:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.36"/>
+  </cols>
+  <sheetData>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 10:31 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t xml:space="preserve">frq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC Akım</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Şarj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float Şarj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devreye al. Akım voltajı kontrol et. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oto şarj test</t>
   </si>
 </sst>
 </file>
@@ -248,15 +263,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:A13"/>
+  <dimension ref="A4:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.44"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,6 +323,29 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 10:46 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -58,7 +58,22 @@
     <t xml:space="preserve">Float Şarj</t>
   </si>
   <si>
-    <t xml:space="preserve">Devreye al. Akım voltajı kontrol et. </t>
+    <t xml:space="preserve">Devreye al. Akım voltajı ölç ve yaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akım voltajı değiştirme menüsüne gel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akım ve voltajı değiştir ve yaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akım ve voltajı ölç ve yaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ölçüm değeri ile ayar değerini karşılaştır.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cihazı kapatıp aç. Ayar değeri duruyor mu kontrol et.</t>
   </si>
   <si>
     <t xml:space="preserve">Oto şarj test</t>
@@ -263,16 +278,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:B20"/>
+  <dimension ref="A4:B27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.8"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,9 +358,39 @@
         <v>12</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>13</v>
+      <c r="B20" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 13:39 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -58,7 +58,13 @@
     <t xml:space="preserve">Float Şarj</t>
   </si>
   <si>
-    <t xml:space="preserve">Devreye al. Akım voltajı ölç ve yaz.</t>
+    <t xml:space="preserve">Bu modu devreye al.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batarya bağla. Hafif yük ver.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akım voltajı ön panelden oku, ölçüm cihazı ile ölç ve yaz.</t>
   </si>
   <si>
     <t xml:space="preserve">Akım voltajı değiştirme menüsüne gel.</t>
@@ -74,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cihazı kapatıp aç. Ayar değeri duruyor mu kontrol et.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost Şarj</t>
   </si>
   <si>
     <t xml:space="preserve">Oto şarj test</t>
@@ -278,10 +287,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:B27"/>
+  <dimension ref="A4:B31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,12 +394,27 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 14:00 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -58,31 +58,55 @@
     <t xml:space="preserve">Float Şarj</t>
   </si>
   <si>
+    <t xml:space="preserve">Ayarlardan bu moda ait voltaj ve akım değerini oku ve yaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost Şarj</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bu modu devreye al.</t>
   </si>
   <si>
+    <t xml:space="preserve">Testleri</t>
+  </si>
+  <si>
     <t xml:space="preserve">Batarya bağla. Hafif yük ver.</t>
   </si>
   <si>
-    <t xml:space="preserve">Akım voltajı ön panelden oku, ölçüm cihazı ile ölç ve yaz.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akım voltajı değiştirme menüsüne gel.</t>
+    <t xml:space="preserve">Şarj voltajını kontrol et. Ön panelden oku, ölçüm cihazı ile ölç ve yaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yükü artırarak akım sınırına gel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akım sınırını kontrol et. Ön panelden oku, ölçüm cihazı ile ölç ve yaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akım ve voltajı değiştirme menüsüne gel.</t>
   </si>
   <si>
     <t xml:space="preserve">Akım ve voltajı değiştir ve yaz.</t>
   </si>
   <si>
+    <t xml:space="preserve">Tekrar akım ve voltajı kontrol et ve yaz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ölçüm değeri ile ayar değerini karşılaştır.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cihazı kapatıp aç. Ayar değeri duruyor mu kontrol et.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Akım ve voltajı ölç ve yaz.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ölçüm değeri ile ayar değerini karşılaştır.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cihazı kapatıp aç. Ayar değeri duruyor mu kontrol et.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boost Şarj</t>
+    <t xml:space="preserve">Otomatik Şarj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float ve boost testleri tamamlanmış varsayılıyor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manuel olarak float şarj moduna geç.</t>
   </si>
   <si>
     <t xml:space="preserve">Oto şarj test</t>
@@ -117,12 +141,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEE6EF"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,8 +189,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -173,6 +207,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFDEE6EF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -287,16 +381,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:B31"/>
+  <dimension ref="A4:B33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.83"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,61 +454,90 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>14</v>
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>15</v>
+      <c r="B20" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>16</v>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>17</v>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>18</v>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>19</v>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>17</v>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>21</v>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 14:09 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -91,25 +91,40 @@
     <t xml:space="preserve">Tekrar akım ve voltajı kontrol et ve yaz.</t>
   </si>
   <si>
+    <t xml:space="preserve">Otomatik Şarj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Float ve boost testleri tamamlanmış varsayılıyor.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ölçüm değeri ile ayar değerini karşılaştır.</t>
   </si>
   <si>
+    <t xml:space="preserve">Manuel olarak float şarj moduna geç.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cihazı kapatıp aç. Ayar değeri duruyor mu kontrol et.</t>
   </si>
   <si>
+    <t xml:space="preserve">Voltaj ve akımı ön panelden oku, ölçüm cihazı ile ölç ve yaz.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Akım ve voltajı ölç ve yaz.</t>
   </si>
   <si>
-    <t xml:space="preserve">Otomatik Şarj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Float ve boost testleri tamamlanmış varsayılıyor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manuel olarak float şarj moduna geç.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oto şarj test</t>
+    <t xml:space="preserve">Otomatik şarja al.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zamanlı Şarj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zamanlı şarj moduna geç.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zamanı 1dk ya ayarla.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana menüye gel.</t>
   </si>
 </sst>
 </file>
@@ -381,10 +396,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:B33"/>
+  <dimension ref="A4:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -506,38 +521,63 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>29</v>
+      <c r="B33" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 15:06 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -125,6 +125,21 @@
   </si>
   <si>
     <t xml:space="preserve">Ana menüye gel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost şarj(Zmn) iletisini oku.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akım ve voltajı ön panelden oku.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yazılı kayıtlardaki boost şarj değerlerine uygun olduğuna bak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akü hattı kopuk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akü sigorta atık ise test yapılmayacak şekilde ayarlandı.</t>
   </si>
 </sst>
 </file>
@@ -396,15 +411,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:E33"/>
+  <dimension ref="A4:E43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.83"/>
   </cols>
   <sheetData>
@@ -578,6 +593,29 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 15:12 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -55,13 +55,13 @@
     <t xml:space="preserve">Şarj</t>
   </si>
   <si>
-    <t xml:space="preserve">Float Şarj</t>
+    <t xml:space="preserve">Normal Şarj</t>
   </si>
   <si>
     <t xml:space="preserve">Ayarlardan bu moda ait voltaj ve akım değerini oku ve yaz.</t>
   </si>
   <si>
-    <t xml:space="preserve">Boost Şarj</t>
+    <t xml:space="preserve">Hızlı Şarj</t>
   </si>
   <si>
     <t xml:space="preserve">Bu modu devreye al.</t>
@@ -94,13 +94,13 @@
     <t xml:space="preserve">Otomatik Şarj</t>
   </si>
   <si>
-    <t xml:space="preserve">Float ve boost testleri tamamlanmış varsayılıyor.</t>
+    <t xml:space="preserve">Normal ve hızlı testleri tamamlanmış varsayılıyor.</t>
   </si>
   <si>
     <t xml:space="preserve">Ölçüm değeri ile ayar değerini karşılaştır.</t>
   </si>
   <si>
-    <t xml:space="preserve">Manuel olarak float şarj moduna geç.</t>
+    <t xml:space="preserve">Manuel olarak normal şarj moduna geç.</t>
   </si>
   <si>
     <t xml:space="preserve">Cihazı kapatıp aç. Ayar değeri duruyor mu kontrol et.</t>
@@ -127,13 +127,22 @@
     <t xml:space="preserve">Ana menüye gel.</t>
   </si>
   <si>
-    <t xml:space="preserve">Boost şarj(Zmn) iletisini oku.</t>
+    <t xml:space="preserve">Hızlı şarj(Zmn) iletisini oku.</t>
   </si>
   <si>
     <t xml:space="preserve">Akım ve voltajı ön panelden oku.</t>
   </si>
   <si>
-    <t xml:space="preserve">Yazılı kayıtlardaki boost şarj değerlerine uygun olduğuna bak.</t>
+    <t xml:space="preserve">Yazılı kayıtlardaki hızlı şarj değerlerine uygun olduğuna bak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sürenin dolmasını bekle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal şarj(Zmn) iletisini oku.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yazılı kayıtlardaki normal şarj değerlerine uygun olduğuna bak.</t>
   </si>
   <si>
     <t xml:space="preserve">Akü hattı kopuk</t>
@@ -414,7 +423,7 @@
   <dimension ref="A4:E43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -610,12 +619,27 @@
         <v>37</v>
       </c>
     </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 15:33 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">Akü sigorta atık ise test yapılmayacak şekilde ayarlandı.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ancak bazen akü sigorta atıkken de test yapıyor.</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:E43"/>
+  <dimension ref="A4:E44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,6 +645,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Auto commit on 2025-06-24 15:42 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hızlı şarj(Zmn) iletisini oku.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalan saniyeyi gösteren sayacı oku.</t>
   </si>
   <si>
     <t xml:space="preserve">Akım ve voltajı ön panelden oku.</t>
@@ -423,10 +426,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:E44"/>
+  <dimension ref="A4:E47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -613,12 +616,12 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="0" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -637,17 +640,37 @@
         <v>40</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="B43" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+      <c r="B46" s="0" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-06-28 05:42 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t xml:space="preserve">Kalibrasyonlar.</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t xml:space="preserve">Yazılı kayıtlardaki normal şarj değerlerine uygun olduğuna bak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cihazı kapatıp aç.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal şarj(Man) iletisini oku.</t>
   </si>
   <si>
     <t xml:space="preserve">Akü hattı kopuk</t>
@@ -426,10 +432,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:E47"/>
+  <dimension ref="A4:E51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -647,7 +653,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,17 +666,37 @@
         <v>36</v>
       </c>
     </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="B46" s="0" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit on 2025-07-08 18:44 - auto
</commit_message>
<xml_diff>
--- a/software_test_proc.xlsx
+++ b/software_test_proc.xlsx
@@ -175,6 +175,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -240,12 +241,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -432,270 +437,270 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:E51"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="62.83"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>0</v>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>4</v>
+      <c r="A8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>5</v>
+      <c r="A9" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>1</v>
+      <c r="A10" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>7</v>
+      <c r="A11" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>8</v>
+      <c r="A13" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>9</v>
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>10</v>
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>16</v>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1" t="s">
-        <v>17</v>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
-        <v>18</v>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="1" t="s">
-        <v>19</v>
+      <c r="B22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="1" t="s">
-        <v>20</v>
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="1" t="s">
-        <v>21</v>
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>24</v>
+      <c r="B29" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>26</v>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>32</v>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>33</v>
+      <c r="B32" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>34</v>
+      <c r="B33" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>35</v>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>36</v>
+      <c r="B35" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>38</v>
+      <c r="B37" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>39</v>
+      <c r="B38" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>40</v>
+      <c r="B39" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
-        <v>41</v>
+      <c r="B40" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
-        <v>35</v>
+      <c r="B42" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
-        <v>36</v>
+      <c r="B43" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
-        <v>26</v>
+      <c r="B44" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="1" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>